<commit_message>
error recognition arduino code
</commit_message>
<xml_diff>
--- a/Sprint3/week5/Group25 DBL Scrum Timesheets.xlsx
+++ b/Sprint3/week5/Group25 DBL Scrum Timesheets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tuenl-my.sharepoint.com/personal/m_topac_student_tue_nl/Documents/Year 1/Q4/2IO75 - DBL Embedded Systems/GitHub Repository/Sprint3/week5/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tuenl-my.sharepoint.com/personal/c_i_zanders_student_tue_nl/Documents/Documents/gitkraken/Embedded_system_group25/Sprint3/week5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{D1C6CDD2-47D0-4AEB-BD27-CCAD9674EF2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F3E91EAB-541C-44D3-B7A8-96D91C21E8D0}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{D1C6CDD2-47D0-4AEB-BD27-CCAD9674EF2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4A079F64-FAE5-4D41-AB78-AD28452877B4}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" r:id="rId1"/>
@@ -1091,7 +1091,7 @@
                   <c:v>1.5840277777777776</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.39583333333333337</c:v>
+                  <c:v>0.95833333333333337</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.70833333333333326</c:v>
@@ -1189,7 +1189,7 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2091029163"/>
@@ -1265,7 +1265,7 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="443840806"/>
@@ -1288,7 +1288,7 @@
               <a:latin typeface="+mn-lt"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-NL"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1329,7 +1329,7 @@
                 <c:formatCode>[h]:mm</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1.7298611111111108</c:v>
+                  <c:v>1.9381944444444443</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.3645833333333333</c:v>
@@ -1338,10 +1338,10 @@
                   <c:v>1.3229166666666665</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.5625</c:v>
+                  <c:v>1.6875</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.21875</c:v>
+                  <c:v>1.4479166666666665</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -1368,7 +1368,7 @@
                 <c:formatCode>[h]:mm</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1.7298611111111108</c:v>
+                  <c:v>1.9381944444444443</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.3645833333333333</c:v>
@@ -1377,10 +1377,10 @@
                   <c:v>1.3229166666666665</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.5625</c:v>
+                  <c:v>1.6875</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.21875</c:v>
+                  <c:v>1.4479166666666665</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -1461,7 +1461,7 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1669176459"/>
@@ -1507,7 +1507,7 @@
               <a:latin typeface="+mn-lt"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-NL"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1926,7 +1926,7 @@
                   <c:v>8.3333333333333329E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.125</c:v>
+                  <c:v>2.541666666666667</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -2017,7 +2017,7 @@
               <a:latin typeface="+mn-lt"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-NL"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4907,7 +4907,7 @@
       <c r="W26" s="39"/>
       <c r="X26" s="39"/>
     </row>
-    <row r="27" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="1"/>
       <c r="B27" s="18" t="str">
         <f t="array" ref="B27">INDEX(Tasks,22,2)</f>
@@ -4935,7 +4935,7 @@
       <c r="W27" s="39"/>
       <c r="X27" s="39"/>
     </row>
-    <row r="28" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="1"/>
       <c r="B28" s="18" t="str">
         <f t="array" ref="B28">INDEX(Tasks,23,2)</f>
@@ -4963,7 +4963,7 @@
       <c r="W28" s="39"/>
       <c r="X28" s="39"/>
     </row>
-    <row r="29" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="1"/>
       <c r="B29" s="18" t="str">
         <f t="array" ref="B29">INDEX(Tasks,24,2)</f>
@@ -9029,7 +9029,7 @@
       <c r="W26" s="39"/>
       <c r="X26" s="39"/>
     </row>
-    <row r="27" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="1"/>
       <c r="B27" s="18" t="str">
         <f t="array" ref="B27">INDEX(Tasks,22,2)</f>
@@ -9057,7 +9057,7 @@
       <c r="W27" s="39"/>
       <c r="X27" s="39"/>
     </row>
-    <row r="28" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="1"/>
       <c r="B28" s="18" t="str">
         <f t="array" ref="B28">INDEX(Tasks,23,2)</f>
@@ -9085,7 +9085,7 @@
       <c r="W28" s="39"/>
       <c r="X28" s="39"/>
     </row>
-    <row r="29" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="1"/>
       <c r="B29" s="18" t="str">
         <f t="array" ref="B29">INDEX(Tasks,24,2)</f>
@@ -9179,7 +9179,7 @@
       <c r="W31" s="39"/>
       <c r="X31" s="39"/>
     </row>
-    <row r="32" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B32" s="18" t="str">
         <f t="array" ref="B32">INDEX(Tasks,27,2)</f>
         <v>Sprint Task 4.5: requesting parts</v>
@@ -9207,7 +9207,7 @@
       <c r="W32" s="39"/>
       <c r="X32" s="39"/>
     </row>
-    <row r="33" spans="2:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B33" s="18" t="str">
         <f t="array" ref="B33">INDEX(Tasks,28,2)</f>
         <v>Belt inspection:</v>
@@ -9235,7 +9235,7 @@
       <c r="W33" s="39"/>
       <c r="X33" s="39"/>
     </row>
-    <row r="34" spans="2:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B34" s="18" t="str">
         <f t="array" ref="B34">INDEX(Tasks,29,2)</f>
         <v>sprint Task 4.6: Fixing the robot manipulator 3D mesh</v>
@@ -9263,7 +9263,7 @@
       <c r="W34" s="39"/>
       <c r="X34" s="39"/>
     </row>
-    <row r="35" spans="2:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B35" s="18">
         <f t="array" ref="B35">INDEX(Tasks,30,2)</f>
         <v>0</v>
@@ -11290,7 +11290,7 @@
       <c r="W122" s="39"/>
       <c r="X122" s="39"/>
     </row>
-    <row r="123" spans="2:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="2:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B123" s="18"/>
       <c r="C123" s="45"/>
       <c r="D123" s="45"/>
@@ -11313,7 +11313,7 @@
       <c r="W123" s="39"/>
       <c r="X123" s="39"/>
     </row>
-    <row r="124" spans="2:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="2:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B124" s="18"/>
       <c r="C124" s="45"/>
       <c r="D124" s="45"/>
@@ -11336,7 +11336,7 @@
       <c r="W124" s="39"/>
       <c r="X124" s="39"/>
     </row>
-    <row r="125" spans="2:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="2:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B125" s="18"/>
       <c r="C125" s="45"/>
       <c r="D125" s="45"/>
@@ -11359,7 +11359,7 @@
       <c r="W125" s="39"/>
       <c r="X125" s="39"/>
     </row>
-    <row r="126" spans="2:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B126" s="18"/>
       <c r="C126" s="45"/>
       <c r="D126" s="45"/>
@@ -11382,7 +11382,7 @@
       <c r="W126" s="39"/>
       <c r="X126" s="39"/>
     </row>
-    <row r="127" spans="2:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B127" s="18"/>
       <c r="C127" s="45"/>
       <c r="D127" s="45"/>
@@ -11405,7 +11405,7 @@
       <c r="W127" s="39"/>
       <c r="X127" s="39"/>
     </row>
-    <row r="128" spans="2:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="2:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B128" s="18" t="s">
         <v>160</v>
       </c>
@@ -11460,7 +11460,7 @@
       <c r="W128" s="39"/>
       <c r="X128" s="39"/>
     </row>
-    <row r="129" spans="2:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="2:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B129" s="18"/>
       <c r="M129" s="47"/>
       <c r="O129" s="39"/>
@@ -13137,7 +13137,7 @@
       <c r="W26" s="39"/>
       <c r="X26" s="39"/>
     </row>
-    <row r="27" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="1"/>
       <c r="B27" s="18" t="str">
         <f t="array" ref="B27">INDEX(Tasks,22,2)</f>
@@ -13165,7 +13165,7 @@
       <c r="W27" s="39"/>
       <c r="X27" s="39"/>
     </row>
-    <row r="28" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="1"/>
       <c r="B28" s="18" t="str">
         <f t="array" ref="B28">INDEX(Tasks,23,2)</f>
@@ -13193,7 +13193,7 @@
       <c r="W28" s="39"/>
       <c r="X28" s="39"/>
     </row>
-    <row r="29" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="1"/>
       <c r="B29" s="18" t="str">
         <f t="array" ref="B29">INDEX(Tasks,24,2)</f>
@@ -17240,7 +17240,7 @@
       <c r="W26" s="39"/>
       <c r="X26" s="39"/>
     </row>
-    <row r="27" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="1"/>
       <c r="B27" s="18" t="str">
         <f t="array" ref="B27">INDEX(Tasks,22,2)</f>
@@ -17268,7 +17268,7 @@
       <c r="W27" s="39"/>
       <c r="X27" s="39"/>
     </row>
-    <row r="28" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="1"/>
       <c r="B28" s="18" t="str">
         <f t="array" ref="B28">INDEX(Tasks,23,2)</f>
@@ -17296,7 +17296,7 @@
       <c r="W28" s="39"/>
       <c r="X28" s="39"/>
     </row>
-    <row r="29" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="1"/>
       <c r="B29" s="18" t="str">
         <f t="array" ref="B29">INDEX(Tasks,24,2)</f>
@@ -17378,7 +17378,7 @@
       <c r="W31" s="39"/>
       <c r="X31" s="39"/>
     </row>
-    <row r="32" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B32" s="18" t="str">
         <f t="array" ref="B32">INDEX(Tasks,27,2)</f>
         <v>Sprint Task 4.5: requesting parts</v>
@@ -17404,7 +17404,7 @@
       <c r="W32" s="39"/>
       <c r="X32" s="39"/>
     </row>
-    <row r="33" spans="2:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B33" s="18" t="str">
         <f t="array" ref="B33">INDEX(Tasks,28,2)</f>
         <v>Belt inspection:</v>
@@ -17430,7 +17430,7 @@
       <c r="W33" s="39"/>
       <c r="X33" s="39"/>
     </row>
-    <row r="34" spans="2:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B34" s="18" t="str">
         <f t="array" ref="B34">INDEX(Tasks,29,2)</f>
         <v>sprint Task 4.6: Fixing the robot manipulator 3D mesh</v>
@@ -17456,7 +17456,7 @@
       <c r="W34" s="39"/>
       <c r="X34" s="39"/>
     </row>
-    <row r="35" spans="2:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B35" s="18">
         <f t="array" ref="B35">INDEX(Tasks,30,2)</f>
         <v>0</v>
@@ -20667,7 +20667,7 @@
   </sheetPr>
   <dimension ref="A1:X1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
@@ -21290,7 +21290,7 @@
       <c r="W26" s="39"/>
       <c r="X26" s="39"/>
     </row>
-    <row r="27" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="1"/>
       <c r="B27" s="18"/>
       <c r="C27" s="10"/>
@@ -21315,7 +21315,7 @@
       <c r="W27" s="39"/>
       <c r="X27" s="39"/>
     </row>
-    <row r="28" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="1"/>
       <c r="B28" s="18"/>
       <c r="C28" s="19"/>
@@ -21340,7 +21340,7 @@
       <c r="W28" s="39"/>
       <c r="X28" s="39"/>
     </row>
-    <row r="29" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="1"/>
       <c r="B29" s="18"/>
       <c r="C29" s="19"/>
@@ -24705,8 +24705,8 @@
   </sheetPr>
   <dimension ref="A1:X1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -24910,15 +24910,21 @@
         <f t="array" ref="B10">INDEX(Tasks,5,2)</f>
         <v>Lectures/Plenary meetings</v>
       </c>
-      <c r="C10" s="14"/>
+      <c r="C10" s="14">
+        <v>0.16666666666666666</v>
+      </c>
       <c r="D10" s="14">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="E10" s="44">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="F10" s="44"/>
-      <c r="G10" s="44"/>
+      <c r="F10" s="44">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="G10" s="44">
+        <v>0.16666666666666666</v>
+      </c>
       <c r="H10" s="44"/>
       <c r="I10" s="11"/>
       <c r="J10" s="44"/>
@@ -24940,15 +24946,21 @@
         <f t="array" ref="B11">INDEX(Tasks,6,2)</f>
         <v>Sprint Tasks</v>
       </c>
-      <c r="C11" s="10"/>
+      <c r="C11" s="14">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="D11" s="14">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="E11" s="44">
         <v>0.14583333333333334</v>
       </c>
-      <c r="F11" s="44"/>
-      <c r="G11" s="44"/>
+      <c r="F11" s="44">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="G11" s="44">
+        <v>6.25E-2</v>
+      </c>
       <c r="H11" s="39"/>
       <c r="I11" s="44"/>
       <c r="J11" s="39"/>
@@ -24970,7 +24982,9 @@
         <f t="array" ref="B12">INDEX(Tasks,7,2)</f>
         <v xml:space="preserve">Sprint Task 1.1: Read course material </v>
       </c>
-      <c r="C12" s="11"/>
+      <c r="C12" s="11">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="D12" s="11"/>
       <c r="E12" s="44"/>
       <c r="F12" s="44"/>
@@ -25356,7 +25370,7 @@
       <c r="W26" s="39"/>
       <c r="X26" s="39"/>
     </row>
-    <row r="27" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="1"/>
       <c r="B27" s="18" t="str">
         <f t="array" ref="B27">INDEX(Tasks,22,2)</f>
@@ -25384,7 +25398,7 @@
       <c r="W27" s="39"/>
       <c r="X27" s="39"/>
     </row>
-    <row r="28" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="1"/>
       <c r="B28" s="18" t="str">
         <f t="array" ref="B28">INDEX(Tasks,23,2)</f>
@@ -25412,7 +25426,7 @@
       <c r="W28" s="39"/>
       <c r="X28" s="39"/>
     </row>
-    <row r="29" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="1"/>
       <c r="B29" s="18" t="str">
         <f t="array" ref="B29">INDEX(Tasks,24,2)</f>
@@ -27720,7 +27734,7 @@
       </c>
       <c r="C128" s="46">
         <f t="shared" ref="C128:L128" si="0">SUM(C5:C127)</f>
-        <v>0</v>
+        <v>0.20833333333333334</v>
       </c>
       <c r="D128" s="46">
         <f t="shared" si="0"/>
@@ -27732,11 +27746,11 @@
       </c>
       <c r="F128" s="46">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.125</v>
       </c>
       <c r="G128" s="46">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.22916666666666666</v>
       </c>
       <c r="H128" s="46">
         <f t="shared" si="0"/>
@@ -27789,43 +27803,43 @@
       </c>
       <c r="C130" s="12">
         <f>SUM(C128)</f>
-        <v>0</v>
+        <v>0.20833333333333334</v>
       </c>
       <c r="D130" s="39">
         <f>SUM(D128,C128)</f>
-        <v>0.16666666666666666</v>
+        <v>0.375</v>
       </c>
       <c r="E130" s="39">
         <f>SUM(E128,C128,D128)</f>
-        <v>0.39583333333333337</v>
+        <v>0.60416666666666663</v>
       </c>
       <c r="F130" s="39">
         <f>SUM(C128:F128)</f>
-        <v>0.39583333333333337</v>
+        <v>0.72916666666666674</v>
       </c>
       <c r="G130" s="39">
         <f>SUM(C128:G128)</f>
-        <v>0.39583333333333337</v>
+        <v>0.95833333333333337</v>
       </c>
       <c r="H130" s="39">
         <f>SUM(C128:H128)</f>
-        <v>0.39583333333333337</v>
+        <v>0.95833333333333337</v>
       </c>
       <c r="I130" s="39">
         <f>SUM(C128:I128)</f>
-        <v>0.39583333333333337</v>
+        <v>0.95833333333333337</v>
       </c>
       <c r="J130" s="39">
         <f>SUM(C128:J128)</f>
-        <v>0.39583333333333337</v>
+        <v>0.95833333333333337</v>
       </c>
       <c r="K130" s="39">
         <f>SUM(C128:K128)</f>
-        <v>0.39583333333333337</v>
+        <v>0.95833333333333337</v>
       </c>
       <c r="L130" s="39">
         <f>SUM(C128:L128)</f>
-        <v>0.39583333333333337</v>
+        <v>0.95833333333333337</v>
       </c>
       <c r="M130" s="47"/>
       <c r="O130" s="39"/>
@@ -27845,43 +27859,43 @@
       </c>
       <c r="C131" s="39">
         <f>Parameters!$G$9-C130</f>
-        <v>5.833333333333333</v>
+        <v>5.625</v>
       </c>
       <c r="D131" s="39">
         <f>Parameters!$G$9-D130</f>
-        <v>5.6666666666666661</v>
+        <v>5.458333333333333</v>
       </c>
       <c r="E131" s="39">
         <f>Parameters!$G$9-E130</f>
-        <v>5.4375</v>
+        <v>5.2291666666666661</v>
       </c>
       <c r="F131" s="39">
         <f>Parameters!$G$9-F130</f>
-        <v>5.4375</v>
+        <v>5.1041666666666661</v>
       </c>
       <c r="G131" s="39">
         <f>Parameters!$G$9-G130</f>
-        <v>5.4375</v>
+        <v>4.875</v>
       </c>
       <c r="H131" s="39">
         <f>Parameters!$G$9-H130</f>
-        <v>5.4375</v>
+        <v>4.875</v>
       </c>
       <c r="I131" s="39">
         <f>Parameters!$G$9-I130</f>
-        <v>5.4375</v>
+        <v>4.875</v>
       </c>
       <c r="J131" s="39">
         <f>Parameters!$G$9-J130</f>
-        <v>5.4375</v>
+        <v>4.875</v>
       </c>
       <c r="K131" s="39">
         <f>Parameters!$G$9-K130</f>
-        <v>5.4375</v>
+        <v>4.875</v>
       </c>
       <c r="L131" s="39">
         <f>Parameters!$G$9-L130</f>
-        <v>5.4375</v>
+        <v>4.875</v>
       </c>
       <c r="O131" s="39"/>
       <c r="P131" s="39"/>
@@ -29064,7 +29078,7 @@
       </c>
       <c r="C10" s="48">
         <f>SUM('Serkan Efe Durusu'!C10,'Ismail Elmasry'!C10,'can Işmar'!C10,'Marios Papalouka'!C10,'Metehan Topaç'!C10,'Celine Zanders '!C10)</f>
-        <v>0.72916666666666663</v>
+        <v>0.89583333333333326</v>
       </c>
       <c r="D10" s="48">
         <f>SUM('Serkan Efe Durusu'!D10,'Ismail Elmasry'!D10,'can Işmar'!D10,'Marios Papalouka'!D10,'Metehan Topaç'!D10,'Celine Zanders '!D10)</f>
@@ -29076,11 +29090,11 @@
       </c>
       <c r="F10" s="48">
         <f>SUM('Serkan Efe Durusu'!F10,'Ismail Elmasry'!F10,'can Işmar'!F10,'Marios Papalouka'!F10,'Metehan Topaç'!F10,'Celine Zanders '!F10)</f>
-        <v>0.25</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="G10" s="48">
         <f>SUM('Serkan Efe Durusu'!G10,'Ismail Elmasry'!G10,'can Işmar'!G10,'Marios Papalouka'!G10,'Metehan Topaç'!G10,'Celine Zanders '!G10)</f>
-        <v>0.29166666666666663</v>
+        <v>0.45833333333333326</v>
       </c>
       <c r="H10" s="48">
         <f>SUM('Serkan Efe Durusu'!H10,'Ismail Elmasry'!H10,'can Işmar'!H10,'Marios Papalouka'!H10,'Metehan Topaç'!H10,'Celine Zanders '!H10)</f>
@@ -29104,7 +29118,7 @@
       </c>
       <c r="M10" s="51">
         <f t="shared" si="0"/>
-        <v>2.125</v>
+        <v>2.541666666666667</v>
       </c>
       <c r="N10" s="50" t="str">
         <f t="array" ref="N10">IF(INDEX(Tasks,1,3)&lt;&gt;"",100*M10/INDEX(Tasks,1,3),"")</f>
@@ -29118,7 +29132,7 @@
       </c>
       <c r="C11" s="48">
         <f>SUM('Serkan Efe Durusu'!C11,'Ismail Elmasry'!C11,'can Işmar'!C11,'Marios Papalouka'!C11,'Metehan Topaç'!D11,'Celine Zanders '!C11)</f>
-        <v>0.39583333333333331</v>
+        <v>0.41666666666666663</v>
       </c>
       <c r="D11" s="48" t="e">
         <f>SUM('Serkan Efe Durusu'!D11,'Ismail Elmasry'!D11,'can Işmar'!D11,'Marios Papalouka'!D11,'Metehan Topaç'!#REF!,'Celine Zanders '!D11)</f>
@@ -29130,11 +29144,11 @@
       </c>
       <c r="F11" s="48">
         <f>SUM('Serkan Efe Durusu'!F11,'Ismail Elmasry'!F11,'can Işmar'!F11,'Marios Papalouka'!F11,'Metehan Topaç'!F11,'Celine Zanders '!F11)</f>
-        <v>0.625</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="G11" s="48">
         <f>SUM('Serkan Efe Durusu'!G11,'Ismail Elmasry'!G11,'can Işmar'!G11,'Marios Papalouka'!G11,'Metehan Topaç'!G11,'Celine Zanders '!G11)</f>
-        <v>0.29166666666666663</v>
+        <v>0.35416666666666663</v>
       </c>
       <c r="H11" s="48">
         <f>SUM('Serkan Efe Durusu'!H11,'Ismail Elmasry'!H11,'can Işmar'!H11,'Marios Papalouka'!H11,'Metehan Topaç'!H11,'Celine Zanders '!H11)</f>
@@ -29172,7 +29186,7 @@
       </c>
       <c r="C12" s="48">
         <f>SUM('Serkan Efe Durusu'!C12,'Ismail Elmasry'!C12,'can Işmar'!C12,'Marios Papalouka'!C12,'Metehan Topaç'!D12,'Celine Zanders '!C12)</f>
-        <v>0.22916666666666666</v>
+        <v>0.25</v>
       </c>
       <c r="D12" s="48" t="e">
         <f>SUM('Serkan Efe Durusu'!D12,'Ismail Elmasry'!D12,'can Işmar'!D12,'Marios Papalouka'!D12,'Metehan Topaç'!#REF!,'Celine Zanders '!D12)</f>
@@ -35168,7 +35182,7 @@
     <row r="130" spans="2:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="131" spans="2:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="132" spans="2:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="133" spans="2:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B133" s="25"/>
     </row>
     <row r="134" spans="2:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -35263,7 +35277,7 @@
       </c>
       <c r="C136" s="26">
         <f>'Celine Zanders '!C128</f>
-        <v>0</v>
+        <v>0.20833333333333334</v>
       </c>
       <c r="D136" s="26">
         <f>'Celine Zanders '!D128</f>
@@ -35275,11 +35289,11 @@
       </c>
       <c r="F136" s="26">
         <f>'Celine Zanders '!F128</f>
-        <v>0</v>
+        <v>0.125</v>
       </c>
       <c r="G136" s="26">
         <f>'Celine Zanders '!G128</f>
-        <v>0</v>
+        <v>0.22916666666666666</v>
       </c>
       <c r="H136" s="26">
         <f>'Celine Zanders '!H128</f>
@@ -35303,7 +35317,7 @@
       </c>
       <c r="M136" s="54">
         <f t="shared" si="1"/>
-        <v>0.39583333333333337</v>
+        <v>0.95833333333333337</v>
       </c>
     </row>
     <row r="137" spans="2:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -35589,7 +35603,7 @@
     <row r="143" spans="2:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C143" s="54">
         <f t="shared" ref="C143:L143" si="2">SUM(C135:C142)</f>
-        <v>1.7298611111111108</v>
+        <v>1.9381944444444443</v>
       </c>
       <c r="D143" s="54">
         <f t="shared" si="2"/>
@@ -35601,11 +35615,11 @@
       </c>
       <c r="F143" s="54">
         <f t="shared" si="2"/>
-        <v>1.5625</v>
+        <v>1.6875</v>
       </c>
       <c r="G143" s="54">
         <f t="shared" si="2"/>
-        <v>1.21875</v>
+        <v>1.4479166666666665</v>
       </c>
       <c r="H143" s="54">
         <f t="shared" si="2"/>
@@ -35629,7 +35643,7 @@
       </c>
       <c r="M143" s="54">
         <f t="shared" si="1"/>
-        <v>7.1986111111111111</v>
+        <v>7.7611111111111111</v>
       </c>
     </row>
     <row r="144" spans="2:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>